<commit_message>
Fix numeric column formatting in data cleaning example
</commit_message>
<xml_diff>
--- a/examples/04_spreadsheets/data_cleaning/tidy_data.xlsx
+++ b/examples/04_spreadsheets/data_cleaning/tidy_data.xlsx
@@ -476,10 +476,10 @@
           <t>Jan</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C2" t="n">
         <v>2019</v>
       </c>
       <c r="D2" s="2" t="n">
@@ -495,10 +495,10 @@
           <t>Feb</t>
         </is>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="B3" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C3" t="n">
         <v>2019</v>
       </c>
       <c r="D3" s="2" t="n">
@@ -514,10 +514,10 @@
           <t>Mar</t>
         </is>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="B4" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C4" t="n">
         <v>2019</v>
       </c>
       <c r="D4" s="2" t="n">
@@ -533,10 +533,10 @@
           <t>Apr</t>
         </is>
       </c>
-      <c r="B5" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="B5" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C5" t="n">
         <v>2019</v>
       </c>
       <c r="D5" s="2" t="n">
@@ -552,10 +552,10 @@
           <t>May</t>
         </is>
       </c>
-      <c r="B6" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="B6" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C6" t="n">
         <v>2019</v>
       </c>
       <c r="D6" s="2" t="n">
@@ -571,10 +571,10 @@
           <t>Jun</t>
         </is>
       </c>
-      <c r="B7" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="B7" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C7" t="n">
         <v>2019</v>
       </c>
       <c r="D7" s="2" t="n">
@@ -590,10 +590,10 @@
           <t>Jul</t>
         </is>
       </c>
-      <c r="B8" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C8" s="2" t="n">
+      <c r="B8" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C8" t="n">
         <v>2019</v>
       </c>
       <c r="D8" s="2" t="n">
@@ -609,10 +609,10 @@
           <t>Aug</t>
         </is>
       </c>
-      <c r="B9" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C9" s="2" t="n">
+      <c r="B9" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C9" t="n">
         <v>2019</v>
       </c>
       <c r="D9" s="2" t="n">
@@ -628,10 +628,10 @@
           <t>Sep</t>
         </is>
       </c>
-      <c r="B10" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C10" s="2" t="n">
+      <c r="B10" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C10" t="n">
         <v>2019</v>
       </c>
       <c r="D10" s="2" t="n">
@@ -647,10 +647,10 @@
           <t>Oct</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="B11" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C11" t="n">
         <v>2019</v>
       </c>
       <c r="D11" s="2" t="n">
@@ -666,10 +666,10 @@
           <t>Nov</t>
         </is>
       </c>
-      <c r="B12" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C12" s="2" t="n">
+      <c r="B12" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C12" t="n">
         <v>2019</v>
       </c>
       <c r="D12" s="2" t="n">
@@ -685,10 +685,10 @@
           <t>Dec</t>
         </is>
       </c>
-      <c r="B13" s="2" t="n">
-        <v>2001</v>
-      </c>
-      <c r="C13" s="2" t="n">
+      <c r="B13" t="n">
+        <v>2001</v>
+      </c>
+      <c r="C13" t="n">
         <v>2019</v>
       </c>
       <c r="D13" s="2" t="n">

</xml_diff>